<commit_message>
Arrow Swipe - Difficulty Added Start
Started applying difficulty constraints to Arrow Swipe.
</commit_message>
<xml_diff>
--- a/X_not unity files for repo though/Battle Games.xlsx
+++ b/X_not unity files for repo though/Battle Games.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jakew\OneDrive\Desktop\Adam\Games\Brain-Games\X_not unity files for repo though\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A153BCF3-FD22-40EF-B0CE-080753007B7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{953BCDDA-AF22-4588-A284-56E6C02C6020}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{9F5EC675-AA23-44B8-8D11-FBB5FDCF1CAE}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
   <si>
     <t xml:space="preserve">Game name </t>
   </si>
@@ -58,9 +58,6 @@
     <t>Types of charges Generated</t>
   </si>
   <si>
-    <t>Difficulty 1</t>
-  </si>
-  <si>
     <t>Swipe in a specified direction based on the color of an arrow</t>
   </si>
   <si>
@@ -76,33 +73,6 @@
     <t>Colors?</t>
   </si>
   <si>
-    <t>Difficulty 2</t>
-  </si>
-  <si>
-    <t>Difficulty 3</t>
-  </si>
-  <si>
-    <t>Difficulty 4</t>
-  </si>
-  <si>
-    <t>Difficulty 5</t>
-  </si>
-  <si>
-    <t>Just green arrows</t>
-  </si>
-  <si>
-    <t>Green + red</t>
-  </si>
-  <si>
-    <t>Multiple of the same arrow</t>
-  </si>
-  <si>
-    <t>Multiple of different arrows, do the middle arrow</t>
-  </si>
-  <si>
-    <t>All the same arrow except 1</t>
-  </si>
-  <si>
     <t>Enemy Interactions</t>
   </si>
   <si>
@@ -125,6 +95,69 @@
   </si>
   <si>
     <t>Change arrow orientation</t>
+  </si>
+  <si>
+    <t>Circular Green Arrows. Swipe in the direction they are pointing.</t>
+  </si>
+  <si>
+    <t>Red Arrows added. Swipe in the direction opposite of their orientation</t>
+  </si>
+  <si>
+    <t>Multiple Different Arrows. Swipe the correct direction of the middle arrow, based on the color of the middle arrow.</t>
+  </si>
+  <si>
+    <t>Blue arrows added. Swipe in a perpendicular direction.</t>
+  </si>
+  <si>
+    <t>All the same arrow except one. Swipe in the direction of that arrow based on the color.</t>
+  </si>
+  <si>
+    <t>Arrow backgrounds can be different shapes besides circles</t>
+  </si>
+  <si>
+    <t>Mechanic 1</t>
+  </si>
+  <si>
+    <t>Mechanic 2</t>
+  </si>
+  <si>
+    <t>Mechanic 3</t>
+  </si>
+  <si>
+    <t>Mechanic 4</t>
+  </si>
+  <si>
+    <t>Mechanic 5</t>
+  </si>
+  <si>
+    <t>Mechanic 6</t>
+  </si>
+  <si>
+    <t>Mechanic 7</t>
+  </si>
+  <si>
+    <t>Mechanic 8</t>
+  </si>
+  <si>
+    <t>Arrow(s) move</t>
+  </si>
+  <si>
+    <t>Multiple Arrows in the same direction on the screen.</t>
+  </si>
+  <si>
+    <t>Arrow Color</t>
+  </si>
+  <si>
+    <t>Arrow Shape</t>
+  </si>
+  <si>
+    <t>Num of Arrows</t>
+  </si>
+  <si>
+    <t>Arrow Formation</t>
+  </si>
+  <si>
+    <t>Arrow Movement</t>
   </si>
 </sst>
 </file>
@@ -146,15 +179,21 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -162,12 +201,48 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -482,10 +557,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6148370-9C93-4AA0-8466-95A8DCEAE153}">
-  <dimension ref="A1:L7"/>
+  <dimension ref="A1:AB35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O5" sqref="O5"/>
+      <selection activeCell="Q7" sqref="Q7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -493,11 +568,14 @@
     <col min="1" max="1" width="12.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="55.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="5" width="5.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="26" bestFit="1" customWidth="1"/>
-    <col min="7" max="11" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.7109375" customWidth="1"/>
+    <col min="7" max="7" width="35.42578125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="4.42578125" customWidth="1"/>
+    <col min="10" max="28" width="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -513,90 +591,568 @@
       <c r="E1" t="s">
         <v>5</v>
       </c>
-      <c r="F1" t="s">
-        <v>6</v>
-      </c>
-      <c r="G1" t="s">
-        <v>7</v>
-      </c>
-      <c r="H1" t="s">
-        <v>13</v>
-      </c>
-      <c r="I1" t="s">
-        <v>14</v>
-      </c>
-      <c r="J1" t="s">
-        <v>15</v>
-      </c>
-      <c r="K1" t="s">
-        <v>16</v>
-      </c>
-      <c r="L1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="H1">
+        <v>0</v>
+      </c>
+      <c r="I1">
+        <v>50</v>
+      </c>
+      <c r="J1">
+        <v>100</v>
+      </c>
+      <c r="K1">
+        <v>150</v>
+      </c>
+      <c r="L1">
+        <v>200</v>
+      </c>
+      <c r="M1">
+        <v>250</v>
+      </c>
+      <c r="N1">
+        <v>300</v>
+      </c>
+      <c r="O1">
+        <v>350</v>
+      </c>
+      <c r="P1">
+        <v>400</v>
+      </c>
+      <c r="Q1">
+        <v>450</v>
+      </c>
+      <c r="R1">
+        <v>500</v>
+      </c>
+      <c r="S1">
+        <v>550</v>
+      </c>
+      <c r="T1">
+        <v>600</v>
+      </c>
+      <c r="U1">
+        <v>650</v>
+      </c>
+      <c r="V1">
+        <v>700</v>
+      </c>
+      <c r="W1">
+        <v>750</v>
+      </c>
+      <c r="X1">
+        <v>800</v>
+      </c>
+      <c r="Y1">
+        <v>850</v>
+      </c>
+      <c r="Z1">
+        <v>900</v>
+      </c>
+      <c r="AA1">
+        <v>950</v>
+      </c>
+      <c r="AB1">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="G2" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
+      <c r="J2" s="3"/>
+      <c r="K2" s="3"/>
+      <c r="L2" s="3"/>
+      <c r="M2" s="3"/>
+      <c r="N2" s="3"/>
+      <c r="O2" s="3"/>
+      <c r="P2" s="3"/>
+      <c r="Q2" s="3"/>
+      <c r="R2" s="3"/>
+      <c r="S2" s="3"/>
+      <c r="T2" s="3"/>
+      <c r="U2" s="3"/>
+      <c r="V2" s="4"/>
+      <c r="W2" s="4"/>
+      <c r="X2" s="4"/>
+      <c r="Y2" s="4"/>
+      <c r="Z2" s="4"/>
+      <c r="AA2" s="4"/>
+      <c r="AB2" s="4"/>
+    </row>
+    <row r="3" spans="1:28" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
       <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" t="s">
         <v>8</v>
       </c>
-      <c r="C3" t="s">
+      <c r="G3" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="H3" s="6"/>
+      <c r="I3" s="6"/>
+      <c r="J3" s="6"/>
+      <c r="K3" s="6"/>
+      <c r="L3" s="6"/>
+      <c r="M3" s="6"/>
+      <c r="N3" s="6"/>
+      <c r="O3" s="6"/>
+      <c r="P3" s="6"/>
+      <c r="Q3" s="6"/>
+      <c r="R3" s="6"/>
+      <c r="S3" s="6"/>
+      <c r="T3" s="6"/>
+      <c r="U3" s="6"/>
+      <c r="V3" s="7"/>
+      <c r="W3" s="7"/>
+      <c r="X3" s="7"/>
+      <c r="Y3" s="7"/>
+      <c r="Z3" s="7"/>
+      <c r="AA3" s="7"/>
+      <c r="AB3" s="7"/>
+    </row>
+    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="G4" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="H4" s="9"/>
+      <c r="I4" s="9"/>
+      <c r="J4" s="10"/>
+      <c r="K4" s="10"/>
+      <c r="L4" s="10"/>
+      <c r="M4" s="10"/>
+      <c r="N4" s="10"/>
+      <c r="O4" s="10"/>
+      <c r="P4" s="10"/>
+      <c r="Q4" s="10"/>
+      <c r="R4" s="10"/>
+      <c r="S4" s="10"/>
+      <c r="T4" s="10"/>
+      <c r="U4" s="10"/>
+      <c r="V4" s="9"/>
+      <c r="W4" s="9"/>
+      <c r="X4" s="9"/>
+      <c r="Y4" s="9"/>
+      <c r="Z4" s="9"/>
+      <c r="AA4" s="9"/>
+      <c r="AB4" s="9"/>
+    </row>
+    <row r="5" spans="1:28" ht="45" x14ac:dyDescent="0.25">
+      <c r="G5" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="H5" s="7"/>
+      <c r="I5" s="7"/>
+      <c r="J5" s="6"/>
+      <c r="K5" s="6"/>
+      <c r="L5" s="6"/>
+      <c r="M5" s="6"/>
+      <c r="N5" s="6"/>
+      <c r="O5" s="6"/>
+      <c r="P5" s="6"/>
+      <c r="Q5" s="6"/>
+      <c r="R5" s="6"/>
+      <c r="S5" s="6"/>
+      <c r="T5" s="6"/>
+      <c r="U5" s="6"/>
+      <c r="V5" s="7"/>
+      <c r="W5" s="7"/>
+      <c r="X5" s="7"/>
+      <c r="Y5" s="7"/>
+      <c r="Z5" s="7"/>
+      <c r="AA5" s="7"/>
+      <c r="AB5" s="7"/>
+    </row>
+    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="G6" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="H6" s="9"/>
+      <c r="I6" s="9"/>
+      <c r="J6" s="9"/>
+      <c r="K6" s="9"/>
+      <c r="L6" s="10"/>
+      <c r="M6" s="10"/>
+      <c r="N6" s="9"/>
+      <c r="O6" s="9"/>
+      <c r="P6" s="9"/>
+      <c r="Q6" s="9"/>
+      <c r="R6" s="10"/>
+      <c r="S6" s="10"/>
+      <c r="T6" s="9"/>
+      <c r="U6" s="9"/>
+      <c r="V6" s="9"/>
+      <c r="W6" s="9"/>
+      <c r="X6" s="9"/>
+      <c r="Y6" s="9"/>
+      <c r="Z6" s="9"/>
+      <c r="AA6" s="9"/>
+      <c r="AB6" s="9"/>
+    </row>
+    <row r="7" spans="1:28" ht="30" x14ac:dyDescent="0.25">
+      <c r="G7" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="H7" s="7"/>
+      <c r="I7" s="7"/>
+      <c r="J7" s="7"/>
+      <c r="K7" s="7"/>
+      <c r="L7" s="6"/>
+      <c r="M7" s="6"/>
+      <c r="N7" s="7"/>
+      <c r="O7" s="7"/>
+      <c r="P7" s="7"/>
+      <c r="Q7" s="7"/>
+      <c r="R7" s="6"/>
+      <c r="S7" s="6"/>
+      <c r="T7" s="7"/>
+      <c r="U7" s="7"/>
+      <c r="V7" s="7"/>
+      <c r="W7" s="7"/>
+      <c r="X7" s="7"/>
+      <c r="Y7" s="7"/>
+      <c r="Z7" s="7"/>
+      <c r="AA7" s="7"/>
+      <c r="AB7" s="7"/>
+    </row>
+    <row r="8" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="G8" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="H8" s="9"/>
+      <c r="I8" s="9"/>
+      <c r="J8" s="9"/>
+      <c r="K8" s="9"/>
+      <c r="L8" s="9"/>
+      <c r="M8" s="9"/>
+      <c r="N8" s="10"/>
+      <c r="O8" s="10"/>
+      <c r="P8" s="9"/>
+      <c r="Q8" s="9"/>
+      <c r="R8" s="10"/>
+      <c r="S8" s="10"/>
+      <c r="T8" s="9"/>
+      <c r="U8" s="9"/>
+      <c r="V8" s="9"/>
+      <c r="W8" s="9"/>
+      <c r="X8" s="9"/>
+      <c r="Y8" s="9"/>
+      <c r="Z8" s="9"/>
+      <c r="AA8" s="9"/>
+      <c r="AB8" s="9"/>
+    </row>
+    <row r="9" spans="1:28" ht="60" x14ac:dyDescent="0.25">
+      <c r="G9" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="H9" s="7"/>
+      <c r="I9" s="7"/>
+      <c r="J9" s="7"/>
+      <c r="K9" s="7"/>
+      <c r="L9" s="7"/>
+      <c r="M9" s="7"/>
+      <c r="N9" s="6"/>
+      <c r="O9" s="6"/>
+      <c r="P9" s="7"/>
+      <c r="Q9" s="7"/>
+      <c r="R9" s="6"/>
+      <c r="S9" s="6"/>
+      <c r="T9" s="7"/>
+      <c r="U9" s="7"/>
+      <c r="V9" s="7"/>
+      <c r="W9" s="7"/>
+      <c r="X9" s="7"/>
+      <c r="Y9" s="7"/>
+      <c r="Z9" s="7"/>
+      <c r="AA9" s="7"/>
+      <c r="AB9" s="7"/>
+    </row>
+    <row r="10" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="G10" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="H10" s="9"/>
+      <c r="I10" s="9"/>
+      <c r="J10" s="9"/>
+      <c r="K10" s="9"/>
+      <c r="L10" s="9"/>
+      <c r="M10" s="9"/>
+      <c r="N10" s="9"/>
+      <c r="O10" s="9"/>
+      <c r="P10" s="10"/>
+      <c r="Q10" s="10"/>
+      <c r="R10" s="10"/>
+      <c r="S10" s="10"/>
+      <c r="T10" s="10"/>
+      <c r="U10" s="10"/>
+      <c r="V10" s="9"/>
+      <c r="W10" s="9"/>
+      <c r="X10" s="9"/>
+      <c r="Y10" s="9"/>
+      <c r="Z10" s="9"/>
+      <c r="AA10" s="9"/>
+      <c r="AB10" s="9"/>
+    </row>
+    <row r="11" spans="1:28" ht="30" x14ac:dyDescent="0.25">
+      <c r="G11" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="H11" s="7"/>
+      <c r="I11" s="7"/>
+      <c r="J11" s="7"/>
+      <c r="K11" s="7"/>
+      <c r="L11" s="7"/>
+      <c r="M11" s="7"/>
+      <c r="N11" s="7"/>
+      <c r="O11" s="7"/>
+      <c r="P11" s="6"/>
+      <c r="Q11" s="6"/>
+      <c r="R11" s="6"/>
+      <c r="S11" s="6"/>
+      <c r="T11" s="6"/>
+      <c r="U11" s="6"/>
+      <c r="V11" s="7"/>
+      <c r="W11" s="7"/>
+      <c r="X11" s="7"/>
+      <c r="Y11" s="7"/>
+      <c r="Z11" s="7"/>
+      <c r="AA11" s="7"/>
+      <c r="AB11" s="7"/>
+    </row>
+    <row r="12" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="G12" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="H12" s="9"/>
+      <c r="I12" s="9"/>
+      <c r="J12" s="9"/>
+      <c r="K12" s="9"/>
+      <c r="L12" s="9"/>
+      <c r="M12" s="9"/>
+      <c r="N12" s="9"/>
+      <c r="O12" s="9"/>
+      <c r="P12" s="9"/>
+      <c r="Q12" s="9"/>
+      <c r="R12" s="10"/>
+      <c r="S12" s="10"/>
+      <c r="T12" s="9"/>
+      <c r="U12" s="9"/>
+      <c r="V12" s="9"/>
+      <c r="W12" s="9"/>
+      <c r="X12" s="9"/>
+      <c r="Y12" s="9"/>
+      <c r="Z12" s="9"/>
+      <c r="AA12" s="9"/>
+      <c r="AB12" s="9"/>
+    </row>
+    <row r="13" spans="1:28" ht="30" x14ac:dyDescent="0.25">
+      <c r="G13" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="D3" t="s">
+      <c r="H13" s="7"/>
+      <c r="I13" s="7"/>
+      <c r="J13" s="7"/>
+      <c r="K13" s="7"/>
+      <c r="L13" s="7"/>
+      <c r="M13" s="7"/>
+      <c r="N13" s="7"/>
+      <c r="O13" s="7"/>
+      <c r="P13" s="7"/>
+      <c r="Q13" s="7"/>
+      <c r="R13" s="6"/>
+      <c r="S13" s="6"/>
+      <c r="T13" s="7"/>
+      <c r="U13" s="7"/>
+      <c r="V13" s="7"/>
+      <c r="W13" s="7"/>
+      <c r="X13" s="7"/>
+      <c r="Y13" s="7"/>
+      <c r="Z13" s="7"/>
+      <c r="AA13" s="7"/>
+      <c r="AB13" s="7"/>
+    </row>
+    <row r="14" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="G14" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="H14" s="9"/>
+      <c r="I14" s="9"/>
+      <c r="J14" s="9"/>
+      <c r="K14" s="9"/>
+      <c r="L14" s="9"/>
+      <c r="M14" s="9"/>
+      <c r="N14" s="9"/>
+      <c r="O14" s="9"/>
+      <c r="P14" s="9"/>
+      <c r="Q14" s="9"/>
+      <c r="R14" s="9"/>
+      <c r="S14" s="9"/>
+      <c r="T14" s="10"/>
+      <c r="U14" s="10"/>
+      <c r="V14" s="9"/>
+      <c r="W14" s="9"/>
+      <c r="X14" s="9"/>
+      <c r="Y14" s="9"/>
+      <c r="Z14" s="9"/>
+      <c r="AA14" s="9"/>
+      <c r="AB14" s="9"/>
+    </row>
+    <row r="15" spans="1:28" ht="45" x14ac:dyDescent="0.25">
+      <c r="G15" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="H15" s="7"/>
+      <c r="I15" s="7"/>
+      <c r="J15" s="7"/>
+      <c r="K15" s="7"/>
+      <c r="L15" s="7"/>
+      <c r="M15" s="7"/>
+      <c r="N15" s="7"/>
+      <c r="O15" s="7"/>
+      <c r="P15" s="7"/>
+      <c r="Q15" s="7"/>
+      <c r="R15" s="7"/>
+      <c r="S15" s="7"/>
+      <c r="T15" s="6"/>
+      <c r="U15" s="6"/>
+      <c r="V15" s="7"/>
+      <c r="W15" s="7"/>
+      <c r="X15" s="7"/>
+      <c r="Y15" s="7"/>
+      <c r="Z15" s="7"/>
+      <c r="AA15" s="7"/>
+      <c r="AB15" s="7"/>
+    </row>
+    <row r="16" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="G16" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="H16" s="9"/>
+      <c r="I16" s="9"/>
+      <c r="J16" s="9"/>
+      <c r="K16" s="9"/>
+      <c r="L16" s="9"/>
+      <c r="M16" s="9"/>
+      <c r="N16" s="9"/>
+      <c r="O16" s="9"/>
+      <c r="P16" s="9"/>
+      <c r="Q16" s="9"/>
+      <c r="R16" s="9"/>
+      <c r="S16" s="9"/>
+      <c r="T16" s="9"/>
+      <c r="U16" s="9"/>
+      <c r="V16" s="9"/>
+      <c r="W16" s="9"/>
+      <c r="X16" s="9"/>
+      <c r="Y16" s="9"/>
+      <c r="Z16" s="9"/>
+      <c r="AA16" s="9"/>
+      <c r="AB16" s="9"/>
+    </row>
+    <row r="17" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="G17" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="H17" s="7"/>
+      <c r="I17" s="7"/>
+      <c r="J17" s="7"/>
+      <c r="K17" s="7"/>
+      <c r="L17" s="7"/>
+      <c r="M17" s="7"/>
+      <c r="N17" s="7"/>
+      <c r="O17" s="7"/>
+      <c r="P17" s="7"/>
+      <c r="Q17" s="7"/>
+      <c r="R17" s="7"/>
+      <c r="S17" s="7"/>
+      <c r="T17" s="7"/>
+      <c r="U17" s="7"/>
+      <c r="V17" s="7"/>
+      <c r="W17" s="7"/>
+      <c r="X17" s="7"/>
+      <c r="Y17" s="7"/>
+      <c r="Z17" s="7"/>
+      <c r="AA17" s="7"/>
+      <c r="AB17" s="7"/>
+    </row>
+    <row r="19" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>6</v>
+      </c>
+      <c r="C19" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="20" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="C20" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="21" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
         <v>9</v>
       </c>
-      <c r="F3" t="s">
+      <c r="C21" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="22" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
         <v>10</v>
       </c>
-      <c r="G3" t="s">
+      <c r="C22" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="23" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>11</v>
+      </c>
+      <c r="C23" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="24" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="25" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
         <v>17</v>
       </c>
-      <c r="H3" t="s">
+    </row>
+    <row r="30" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="32" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
         <v>18</v>
-      </c>
-      <c r="I3" t="s">
-        <v>19</v>
-      </c>
-      <c r="J3" t="s">
-        <v>20</v>
-      </c>
-      <c r="K3" t="s">
-        <v>21</v>
-      </c>
-      <c r="L3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="F4" t="s">
-        <v>11</v>
-      </c>
-      <c r="L4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="F5" t="s">
-        <v>12</v>
-      </c>
-      <c r="L5" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="F6" t="s">
-        <v>26</v>
-      </c>
-      <c r="L6" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="F7" t="s">
-        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>